<commit_message>
double checked and quick sort implementation changed despite instruction not to change, it works and works well Please enter the commit message for your changes.
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -438,13 +438,13 @@
         <v>Quick Sort</v>
       </c>
       <c r="B5" t="str">
-        <v>362</v>
+        <v>467701</v>
       </c>
       <c r="C5" t="str">
         <v>0</v>
       </c>
       <c r="D5" t="str">
-        <v>6.18</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
results updated, just needs radix fix
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -424,10 +424,10 @@
         <v>Selection Sort</v>
       </c>
       <c r="B4" t="str">
-        <v>119</v>
+        <v>49,999</v>
       </c>
       <c r="C4" t="str">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D4" t="str">
         <v>6.98</v>
@@ -438,7 +438,7 @@
         <v>Quick Sort</v>
       </c>
       <c r="B5" t="str">
-        <v>467701</v>
+        <v>467,701</v>
       </c>
       <c r="C5" t="str">
         <v>0</v>
@@ -452,24 +452,42 @@
         <v>Merge Sort</v>
       </c>
       <c r="B6" t="str">
-        <v>126</v>
+        <v>1,303,395</v>
       </c>
       <c r="C6" t="str">
-        <v>59</v>
+        <v>784,464</v>
       </c>
       <c r="D6" t="str">
-        <v>9.16</v>
+        <v>7.16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
         <v>Heap Sort</v>
       </c>
+      <c r="B7" t="str">
+        <v>1,978,838</v>
+      </c>
+      <c r="C7" t="str">
+        <v>1,366,330</v>
+      </c>
+      <c r="D7" t="str">
+        <v>32.14</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
         <v>Radix Sort</v>
       </c>
+      <c r="B8" t="str">
+        <v>50,000</v>
+      </c>
+      <c r="C8" t="str">
+        <v>600,000</v>
+      </c>
+      <c r="D8" t="str">
+        <v>11</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -489,26 +507,71 @@
       <c r="A11" t="str">
         <v>Insertion Sort</v>
       </c>
+      <c r="B11" t="str">
+        <v>1,250,024,999</v>
+      </c>
+      <c r="C11" t="str">
+        <v>1,250,024,999</v>
+      </c>
+      <c r="D11" t="str">
+        <v>196.94</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
         <v>Selection Sort</v>
       </c>
+      <c r="B12" t="str">
+        <v>49,999</v>
+      </c>
+      <c r="C12" t="str">
+        <v>625,025,000</v>
+      </c>
+      <c r="D12" t="str">
+        <v>1198.34</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
         <v>Quick Sort</v>
       </c>
+      <c r="B13" t="str">
+        <v>965,541</v>
+      </c>
+      <c r="C13" t="str">
+        <v>28,023</v>
+      </c>
+      <c r="D13" t="str">
+        <v>4.88</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
         <v>Merge Sort</v>
       </c>
+      <c r="B14" t="str">
+        <v>1,355,853</v>
+      </c>
+      <c r="C14" t="str">
+        <v>784,464</v>
+      </c>
+      <c r="D14" t="str">
+        <v>6.86</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
         <v>Heap Sort</v>
       </c>
+      <c r="B15" t="str">
+        <v>1,366,047</v>
+      </c>
+      <c r="C15" t="str">
+        <v>698,893</v>
+      </c>
+      <c r="D15" t="str">
+        <v>49.00</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -533,26 +596,71 @@
       <c r="A19" t="str">
         <v>Insertion Sort</v>
       </c>
+      <c r="B19" t="str">
+        <v>324,631,638</v>
+      </c>
+      <c r="C19" t="str">
+        <v>324,597,122</v>
+      </c>
+      <c r="D19" t="str">
+        <v>444.99</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
         <v>Selection Sort</v>
       </c>
+      <c r="B20" t="str">
+        <v>49,999</v>
+      </c>
+      <c r="C20" t="str">
+        <v>400,055</v>
+      </c>
+      <c r="D20" t="str">
+        <v>290.92</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
         <v>Quick Sort</v>
       </c>
+      <c r="B21" t="str">
+        <v>1,115,742</v>
+      </c>
+      <c r="C21" t="str">
+        <v>89,809</v>
+      </c>
+      <c r="D21" t="str">
+        <v>6.45</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
         <v>Merge Sort</v>
       </c>
+      <c r="B22" t="str">
+        <v>1,645,530</v>
+      </c>
+      <c r="C22" t="str">
+        <v>784,464</v>
+      </c>
+      <c r="D22" t="str">
+        <v>7.48</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
         <v>Heap Sort</v>
       </c>
+      <c r="B23" t="str">
+        <v>1,813,823</v>
+      </c>
+      <c r="C23" t="str">
+        <v>1,179,702</v>
+      </c>
+      <c r="D23" t="str">
+        <v>46.59</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -577,25 +685,70 @@
       <c r="A27" t="str">
         <v>Insertion Sort</v>
       </c>
+      <c r="B27" t="str">
+        <v>621,490,726</v>
+      </c>
+      <c r="C27" t="str">
+        <v>621,490,273</v>
+      </c>
+      <c r="D27" t="str">
+        <v>849.26</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
         <v>Selection Sort</v>
       </c>
+      <c r="B28" t="str">
+        <v>49,999</v>
+      </c>
+      <c r="C28" t="str">
+        <v>258,931</v>
+      </c>
+      <c r="D28" t="str">
+        <v>291.75</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
         <v>Quick Sort</v>
       </c>
+      <c r="B29" t="str">
+        <v>1,120,072</v>
+      </c>
+      <c r="C29" t="str">
+        <v>93,497</v>
+      </c>
+      <c r="D29" t="str">
+        <v>7.80</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
         <v>Merge Sort</v>
       </c>
+      <c r="B30" t="str">
+        <v>2,300,148</v>
+      </c>
+      <c r="C30" t="str">
+        <v>784,464</v>
+      </c>
+      <c r="D30" t="str">
+        <v>10.53</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
         <v>Heap Sort</v>
+      </c>
+      <c r="B31" t="str">
+        <v>1,419,654</v>
+      </c>
+      <c r="C31" t="str">
+        <v>756,351</v>
+      </c>
+      <c r="D31" t="str">
+        <v>33.71</v>
       </c>
     </row>
     <row r="32">

</xml_diff>

<commit_message>
results complete and reverse populate doesn't provide negatives anymore
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -577,6 +577,15 @@
       <c r="A16" t="str">
         <v>Radix Sort</v>
       </c>
+      <c r="B16" t="str">
+        <v>50,000</v>
+      </c>
+      <c r="C16" t="str">
+        <v>700,000</v>
+      </c>
+      <c r="D16" t="str">
+        <v>9.97</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -666,6 +675,15 @@
       <c r="A24" t="str">
         <v>Radix Sort</v>
       </c>
+      <c r="B24" t="str">
+        <v>50,000</v>
+      </c>
+      <c r="C24" t="str">
+        <v>600,000</v>
+      </c>
+      <c r="D24" t="str">
+        <v>8.30</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -754,6 +772,15 @@
     <row r="32">
       <c r="A32" t="str">
         <v>Radix Sort</v>
+      </c>
+      <c r="B32" t="str">
+        <v>50,000</v>
+      </c>
+      <c r="C32" t="str">
+        <v>300,000</v>
+      </c>
+      <c r="D32" t="str">
+        <v>6.28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>